<commit_message>
update and add files
</commit_message>
<xml_diff>
--- a/data-sys-docs/PTAGIS/Data Specifications MRR Excel.xlsx
+++ b/data-sys-docs/PTAGIS/Data Specifications MRR Excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edlabola\code\fish-data-comp\PTAGIS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edlabola\code\fish-data-comp\data-sys-docs\PTAGIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A5608D-427C-4605-B486-EC32359DD6AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB8E94E5-2627-4A41-8B0C-3CF79F1D220D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{50E88988-7DEF-4C96-9044-C4A3CEDEAB59}"/>
+    <workbookView xWindow="84" yWindow="132" windowWidth="12000" windowHeight="11856" activeTab="2" xr2:uid="{50E88988-7DEF-4C96-9044-C4A3CEDEAB59}"/>
   </bookViews>
   <sheets>
     <sheet name="Session" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="257">
   <si>
     <t>Field Name</t>
   </si>
@@ -1226,70 +1226,70 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1612,8 +1612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3602AE8E-1EF0-47F5-AC91-8ACE71C388E3}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1959,7 +1959,7 @@
       </c>
       <c r="J16" s="31"/>
     </row>
-    <row r="17" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="28" t="s">
         <v>47</v>
       </c>
@@ -2014,8 +2014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E77E44E-930A-4725-B518-33F4C7096CA5}">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2319,19 +2319,19 @@
       <c r="E10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="71" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="71" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" s="71" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" s="71" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10" s="68"/>
+      <c r="F10" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="61"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="70"/>
@@ -2341,11 +2341,11 @@
       <c r="E11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="74"/>
-      <c r="G11" s="74"/>
-      <c r="H11" s="74"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="73"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="62"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="70"/>
@@ -2355,11 +2355,11 @@
       <c r="E12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="74"/>
-      <c r="G12" s="74"/>
-      <c r="H12" s="74"/>
-      <c r="I12" s="74"/>
-      <c r="J12" s="73"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="59"/>
+      <c r="J12" s="62"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="70"/>
@@ -2369,11 +2369,11 @@
       <c r="E13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="74"/>
-      <c r="G13" s="74"/>
-      <c r="H13" s="74"/>
-      <c r="I13" s="74"/>
-      <c r="J13" s="73"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="59"/>
+      <c r="J13" s="62"/>
     </row>
     <row r="14" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="65"/>
@@ -2383,11 +2383,11 @@
       <c r="E14" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="F14" s="72"/>
-      <c r="G14" s="72"/>
-      <c r="H14" s="72"/>
-      <c r="I14" s="72"/>
-      <c r="J14" s="69"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="63"/>
     </row>
     <row r="15" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
@@ -2465,19 +2465,19 @@
       <c r="E17" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="F17" s="58" t="s">
-        <v>51</v>
-      </c>
-      <c r="G17" s="58" t="s">
-        <v>51</v>
-      </c>
-      <c r="H17" s="66" t="s">
+      <c r="F17" s="66" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" s="66" t="s">
+        <v>51</v>
+      </c>
+      <c r="H17" s="68" t="s">
         <v>55</v>
       </c>
-      <c r="I17" s="58" t="s">
-        <v>51</v>
-      </c>
-      <c r="J17" s="68"/>
+      <c r="I17" s="66" t="s">
+        <v>51</v>
+      </c>
+      <c r="J17" s="61"/>
     </row>
     <row r="18" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="65"/>
@@ -2487,11 +2487,11 @@
       <c r="E18" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="F18" s="60"/>
-      <c r="G18" s="60"/>
-      <c r="H18" s="67"/>
-      <c r="I18" s="60"/>
-      <c r="J18" s="69"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="67"/>
+      <c r="J18" s="63"/>
     </row>
     <row r="19" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
@@ -2541,19 +2541,19 @@
       <c r="E20" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="F20" s="71" t="s">
-        <v>23</v>
-      </c>
-      <c r="G20" s="71" t="s">
-        <v>23</v>
-      </c>
-      <c r="H20" s="71" t="s">
-        <v>23</v>
-      </c>
-      <c r="I20" s="71" t="s">
-        <v>23</v>
-      </c>
-      <c r="J20" s="68"/>
+      <c r="F20" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="I20" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="J20" s="61"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="70"/>
@@ -2563,11 +2563,11 @@
       <c r="E21" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="F21" s="74"/>
-      <c r="G21" s="74"/>
-      <c r="H21" s="74"/>
-      <c r="I21" s="74"/>
-      <c r="J21" s="73"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="59"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="59"/>
+      <c r="J21" s="62"/>
     </row>
     <row r="22" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="65"/>
@@ -2577,11 +2577,11 @@
       <c r="E22" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="F22" s="72"/>
-      <c r="G22" s="72"/>
-      <c r="H22" s="72"/>
-      <c r="I22" s="72"/>
-      <c r="J22" s="69"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="60"/>
+      <c r="I22" s="60"/>
+      <c r="J22" s="63"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="64" t="s">
@@ -2599,19 +2599,19 @@
       <c r="E23" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="F23" s="61" t="s">
+      <c r="F23" s="71" t="s">
         <v>119</v>
       </c>
-      <c r="G23" s="61" t="s">
+      <c r="G23" s="71" t="s">
         <v>119</v>
       </c>
-      <c r="H23" s="61" t="s">
+      <c r="H23" s="71" t="s">
         <v>119</v>
       </c>
-      <c r="I23" s="61" t="s">
+      <c r="I23" s="71" t="s">
         <v>119</v>
       </c>
-      <c r="J23" s="68"/>
+      <c r="J23" s="61"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="70"/>
@@ -2621,11 +2621,11 @@
       <c r="E24" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="F24" s="62"/>
-      <c r="G24" s="62"/>
-      <c r="H24" s="62"/>
-      <c r="I24" s="62"/>
-      <c r="J24" s="73"/>
+      <c r="F24" s="72"/>
+      <c r="G24" s="72"/>
+      <c r="H24" s="72"/>
+      <c r="I24" s="72"/>
+      <c r="J24" s="62"/>
     </row>
     <row r="25" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="65"/>
@@ -2635,11 +2635,11 @@
       <c r="E25" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="F25" s="63"/>
-      <c r="G25" s="63"/>
-      <c r="H25" s="63"/>
-      <c r="I25" s="63"/>
-      <c r="J25" s="69"/>
+      <c r="F25" s="73"/>
+      <c r="G25" s="73"/>
+      <c r="H25" s="73"/>
+      <c r="I25" s="73"/>
+      <c r="J25" s="63"/>
     </row>
     <row r="26" spans="1:10" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
@@ -2747,19 +2747,19 @@
       <c r="E29" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="F29" s="71" t="s">
-        <v>23</v>
-      </c>
-      <c r="G29" s="71" t="s">
-        <v>23</v>
-      </c>
-      <c r="H29" s="66" t="s">
+      <c r="F29" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="H29" s="68" t="s">
         <v>55</v>
       </c>
-      <c r="I29" s="66" t="s">
+      <c r="I29" s="68" t="s">
         <v>55</v>
       </c>
-      <c r="J29" s="68"/>
+      <c r="J29" s="61"/>
     </row>
     <row r="30" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="65"/>
@@ -2769,11 +2769,11 @@
       <c r="E30" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="F30" s="72"/>
-      <c r="G30" s="72"/>
-      <c r="H30" s="67"/>
-      <c r="I30" s="67"/>
-      <c r="J30" s="69"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="69"/>
+      <c r="I30" s="69"/>
+      <c r="J30" s="63"/>
     </row>
     <row r="31" spans="1:10" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
@@ -3035,16 +3035,16 @@
       <c r="E39" s="64" t="s">
         <v>178</v>
       </c>
-      <c r="F39" s="61" t="s">
+      <c r="F39" s="71" t="s">
         <v>173</v>
       </c>
-      <c r="G39" s="61" t="s">
+      <c r="G39" s="71" t="s">
         <v>173</v>
       </c>
-      <c r="H39" s="58" t="s">
-        <v>51</v>
-      </c>
-      <c r="I39" s="61" t="s">
+      <c r="H39" s="66" t="s">
+        <v>51</v>
+      </c>
+      <c r="I39" s="71" t="s">
         <v>173</v>
       </c>
       <c r="J39" s="9" t="s">
@@ -3057,10 +3057,10 @@
       <c r="C40" s="70"/>
       <c r="D40" s="70"/>
       <c r="E40" s="70"/>
-      <c r="F40" s="62"/>
-      <c r="G40" s="62"/>
-      <c r="H40" s="59"/>
-      <c r="I40" s="62"/>
+      <c r="F40" s="72"/>
+      <c r="G40" s="72"/>
+      <c r="H40" s="74"/>
+      <c r="I40" s="72"/>
       <c r="J40" s="22"/>
     </row>
     <row r="41" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.35">
@@ -3069,10 +3069,10 @@
       <c r="C41" s="65"/>
       <c r="D41" s="65"/>
       <c r="E41" s="65"/>
-      <c r="F41" s="63"/>
-      <c r="G41" s="63"/>
-      <c r="H41" s="60"/>
-      <c r="I41" s="63"/>
+      <c r="F41" s="73"/>
+      <c r="G41" s="73"/>
+      <c r="H41" s="67"/>
+      <c r="I41" s="73"/>
       <c r="J41" s="23" t="s">
         <v>179</v>
       </c>
@@ -3093,16 +3093,16 @@
       <c r="E42" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="F42" s="61" t="s">
+      <c r="F42" s="71" t="s">
         <v>173</v>
       </c>
-      <c r="G42" s="61" t="s">
+      <c r="G42" s="71" t="s">
         <v>173</v>
       </c>
-      <c r="H42" s="66" t="s">
+      <c r="H42" s="68" t="s">
         <v>55</v>
       </c>
-      <c r="I42" s="61" t="s">
+      <c r="I42" s="71" t="s">
         <v>173</v>
       </c>
       <c r="J42" s="52" t="s">
@@ -3117,10 +3117,10 @@
       <c r="E43" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="F43" s="63"/>
-      <c r="G43" s="63"/>
-      <c r="H43" s="67"/>
-      <c r="I43" s="63"/>
+      <c r="F43" s="73"/>
+      <c r="G43" s="73"/>
+      <c r="H43" s="69"/>
+      <c r="I43" s="73"/>
       <c r="J43" s="54"/>
     </row>
     <row r="44" spans="1:10" ht="79.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -3441,6 +3441,53 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="J42:J43"/>
+    <mergeCell ref="H39:H41"/>
+    <mergeCell ref="I39:I41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="G42:G43"/>
+    <mergeCell ref="H42:H43"/>
+    <mergeCell ref="I42:I43"/>
+    <mergeCell ref="F39:F41"/>
+    <mergeCell ref="G39:G41"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="G23:G25"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="I23:I25"/>
+    <mergeCell ref="J23:J25"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="I29:I30"/>
+    <mergeCell ref="J29:J30"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="I20:I22"/>
+    <mergeCell ref="J20:J22"/>
     <mergeCell ref="H10:H14"/>
     <mergeCell ref="I10:I14"/>
     <mergeCell ref="J10:J14"/>
@@ -3457,53 +3504,6 @@
     <mergeCell ref="D10:D14"/>
     <mergeCell ref="F10:F14"/>
     <mergeCell ref="G10:G14"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="G20:G22"/>
-    <mergeCell ref="H20:H22"/>
-    <mergeCell ref="I20:I22"/>
-    <mergeCell ref="J20:J22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="G23:G25"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="I23:I25"/>
-    <mergeCell ref="J23:J25"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="I29:I30"/>
-    <mergeCell ref="J29:J30"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="F39:F41"/>
-    <mergeCell ref="G39:G41"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="J42:J43"/>
-    <mergeCell ref="H39:H41"/>
-    <mergeCell ref="I39:I41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="G42:G43"/>
-    <mergeCell ref="H42:H43"/>
-    <mergeCell ref="I42:I43"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F1" r:id="rId1" display="https://www.ptagis.org/Content/DataSpecification/topics/mark-event.htm" xr:uid="{D36B749B-6EE6-415F-97FD-00123CBE6FED}"/>
@@ -3519,10 +3519,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9079CFF6-228B-405A-9324-4A2F77EAB632}">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3641,10 +3641,10 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="77" t="s">
+      <c r="A8" s="75" t="s">
         <v>108</v>
       </c>
-      <c r="B8" s="77" t="s">
+      <c r="B8" s="75" t="s">
         <v>109</v>
       </c>
       <c r="C8" s="37" t="s">
@@ -3655,8 +3655,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="78"/>
-      <c r="B9" s="78"/>
+      <c r="A9" s="76"/>
+      <c r="B9" s="76"/>
       <c r="C9" s="38" t="s">
         <v>111</v>
       </c>
@@ -3665,8 +3665,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="79"/>
-      <c r="B10" s="79"/>
+      <c r="A10" s="77"/>
+      <c r="B10" s="77"/>
       <c r="C10" s="39" t="s">
         <v>112</v>
       </c>
@@ -3689,10 +3689,10 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="77" t="s">
+      <c r="A12" s="75" t="s">
         <v>136</v>
       </c>
-      <c r="B12" s="77" t="s">
+      <c r="B12" s="75" t="s">
         <v>138</v>
       </c>
       <c r="C12" s="37" t="s">
@@ -3703,8 +3703,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="79"/>
-      <c r="B13" s="79"/>
+      <c r="A13" s="77"/>
+      <c r="B13" s="77"/>
       <c r="C13" s="39" t="s">
         <v>102</v>
       </c>
@@ -3754,7 +3754,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="35" t="s">
         <v>216</v>
       </c>
@@ -3768,217 +3768,220 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="26" t="s">
-        <v>227</v>
-      </c>
-      <c r="B18" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="26" t="s">
-        <v>4</v>
+    <row r="18" spans="1:5" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="B18" s="41" t="s">
+        <v>171</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>237</v>
       </c>
       <c r="D18" s="38" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="41" t="s">
-        <v>170</v>
-      </c>
-      <c r="B19" s="41" t="s">
-        <v>171</v>
-      </c>
-      <c r="C19" s="36" t="s">
-        <v>237</v>
+    <row r="19" spans="1:5" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>178</v>
       </c>
       <c r="D19" s="38" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="28" t="s">
-        <v>176</v>
-      </c>
-      <c r="B20" s="28" t="s">
-        <v>177</v>
-      </c>
-      <c r="C20" s="28" t="s">
-        <v>178</v>
+    <row r="20" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="78" t="s">
+        <v>181</v>
+      </c>
+      <c r="B20" s="78" t="s">
+        <v>183</v>
+      </c>
+      <c r="C20" s="42" t="s">
+        <v>101</v>
       </c>
       <c r="D20" s="38" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="75" t="s">
-        <v>181</v>
-      </c>
-      <c r="B21" s="75" t="s">
-        <v>183</v>
-      </c>
-      <c r="C21" s="42" t="s">
-        <v>101</v>
+    <row r="21" spans="1:5" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="79"/>
+      <c r="B21" s="79"/>
+      <c r="C21" s="43" t="s">
+        <v>102</v>
       </c>
       <c r="D21" s="38" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="76"/>
-      <c r="B22" s="76"/>
-      <c r="C22" s="43" t="s">
+    <row r="22" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" s="44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="D28" s="44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="64" t="s">
+        <v>98</v>
+      </c>
+      <c r="B29" s="64" t="s">
+        <v>239</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" s="44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="65"/>
+      <c r="B30" s="65"/>
+      <c r="C30" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="D22" s="38" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="44" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D24" s="44" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="B25" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="44" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="D26" s="44" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="B27" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="C27" s="35" t="s">
-        <v>75</v>
-      </c>
-      <c r="D27" s="44" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D28" s="44" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="B29" s="35" t="s">
-        <v>95</v>
-      </c>
-      <c r="C29" s="35" t="s">
-        <v>96</v>
-      </c>
-      <c r="D29" s="44" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="64" t="s">
-        <v>98</v>
-      </c>
-      <c r="B30" s="64" t="s">
-        <v>239</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>101</v>
-      </c>
       <c r="D30" s="44" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="65"/>
-      <c r="B31" s="65"/>
-      <c r="C31" s="8" t="s">
-        <v>102</v>
+    <row r="31" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="B31" s="35" t="s">
+        <v>241</v>
+      </c>
+      <c r="C31" s="35" t="s">
+        <v>123</v>
       </c>
       <c r="D31" s="44" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="35" t="s">
-        <v>240</v>
-      </c>
-      <c r="B32" s="35" t="s">
-        <v>241</v>
-      </c>
-      <c r="C32" s="35" t="s">
-        <v>123</v>
+    <row r="32" spans="1:5" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>128</v>
       </c>
       <c r="D32" s="44" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="10" t="s">
-        <v>242</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>128</v>
+      <c r="E32" s="16" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="75" t="s">
+        <v>244</v>
+      </c>
+      <c r="B33" s="75" t="s">
+        <v>115</v>
+      </c>
+      <c r="C33" s="37" t="s">
+        <v>116</v>
       </c>
       <c r="D33" s="44" t="s">
         <v>51</v>
@@ -3987,216 +3990,199 @@
         <v>247</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="77" t="s">
-        <v>244</v>
-      </c>
-      <c r="B34" s="77" t="s">
-        <v>115</v>
-      </c>
-      <c r="C34" s="37" t="s">
-        <v>116</v>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="76"/>
+      <c r="B34" s="76"/>
+      <c r="C34" s="38" t="s">
+        <v>117</v>
       </c>
       <c r="D34" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="E34" s="16" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="78"/>
-      <c r="B35" s="78"/>
-      <c r="C35" s="38" t="s">
-        <v>117</v>
+    </row>
+    <row r="35" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="77"/>
+      <c r="B35" s="77"/>
+      <c r="C35" s="39" t="s">
+        <v>118</v>
       </c>
       <c r="D35" s="44" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="79"/>
-      <c r="B36" s="79"/>
-      <c r="C36" s="39" t="s">
-        <v>118</v>
+      <c r="A36" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>105</v>
       </c>
       <c r="D36" s="44" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="C37" s="10" t="s">
+    <row r="37" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="B37" s="35" t="s">
+        <v>245</v>
+      </c>
+      <c r="C37" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" s="44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="D38" s="44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="35" t="s">
+        <v>162</v>
+      </c>
+      <c r="B39" s="35" t="s">
+        <v>163</v>
+      </c>
+      <c r="C39" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" s="44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="D40" s="44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="35" t="s">
+        <v>198</v>
+      </c>
+      <c r="B41" s="35" t="s">
+        <v>199</v>
+      </c>
+      <c r="C41" s="35" t="s">
+        <v>246</v>
+      </c>
+      <c r="D41" s="44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="D42" s="44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="35" t="s">
+        <v>205</v>
+      </c>
+      <c r="B43" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="C43" s="35" t="s">
+        <v>207</v>
+      </c>
+      <c r="D43" s="44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D44" s="44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="35" t="s">
+        <v>220</v>
+      </c>
+      <c r="B45" s="35" t="s">
+        <v>222</v>
+      </c>
+      <c r="C45" s="35" t="s">
+        <v>223</v>
+      </c>
+      <c r="D45" s="44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="C46" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D37" s="44" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="35" t="s">
-        <v>148</v>
-      </c>
-      <c r="B38" s="35" t="s">
-        <v>245</v>
-      </c>
-      <c r="C38" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="D38" s="44" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="D39" s="44" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="35" t="s">
-        <v>162</v>
-      </c>
-      <c r="B40" s="35" t="s">
-        <v>163</v>
-      </c>
-      <c r="C40" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="D40" s="44" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="D41" s="44" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="35" t="s">
-        <v>198</v>
-      </c>
-      <c r="B42" s="35" t="s">
-        <v>199</v>
-      </c>
-      <c r="C42" s="35" t="s">
-        <v>246</v>
-      </c>
-      <c r="D42" s="44" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="D43" s="44" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="35" t="s">
-        <v>205</v>
-      </c>
-      <c r="B44" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="C44" s="35" t="s">
-        <v>207</v>
-      </c>
-      <c r="D44" s="44" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="C45" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="D45" s="44" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="35" t="s">
-        <v>220</v>
-      </c>
-      <c r="B46" s="35" t="s">
-        <v>222</v>
-      </c>
-      <c r="C46" s="35" t="s">
-        <v>223</v>
-      </c>
       <c r="D46" s="44" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="B47" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="C47" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D47" s="44" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D48" s="44"/>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D47" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="B33:B35"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C6" r:id="rId1" display="https://www.ptagis.org/Content/DataSpecification/topics/timestamps.htm" xr:uid="{2CECE92E-01A6-428D-9B67-AB40EB960975}"/>
-    <hyperlink ref="C19" r:id="rId2" display="https://www.ptagis.org/Content/DataSpecification/topics/timestamps.htm" xr:uid="{F088CBD3-59C5-4E0B-AC12-C40E25535647}"/>
+    <hyperlink ref="C18" r:id="rId2" display="https://www.ptagis.org/Content/DataSpecification/topics/timestamps.htm" xr:uid="{F088CBD3-59C5-4E0B-AC12-C40E25535647}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4326,10 +4312,10 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="77" t="s">
+      <c r="A8" s="75" t="s">
         <v>108</v>
       </c>
-      <c r="B8" s="77" t="s">
+      <c r="B8" s="75" t="s">
         <v>109</v>
       </c>
       <c r="C8" s="37" t="s">
@@ -4340,8 +4326,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="78"/>
-      <c r="B9" s="78"/>
+      <c r="A9" s="76"/>
+      <c r="B9" s="76"/>
       <c r="C9" s="38" t="s">
         <v>111</v>
       </c>
@@ -4350,8 +4336,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="79"/>
-      <c r="B10" s="79"/>
+      <c r="A10" s="77"/>
+      <c r="B10" s="77"/>
       <c r="C10" s="39" t="s">
         <v>112</v>
       </c>
@@ -4468,10 +4454,10 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="75" t="s">
+      <c r="A19" s="78" t="s">
         <v>181</v>
       </c>
-      <c r="B19" s="75" t="s">
+      <c r="B19" s="78" t="s">
         <v>183</v>
       </c>
       <c r="C19" s="42" t="s">
@@ -4482,8 +4468,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="76"/>
-      <c r="B20" s="76"/>
+      <c r="A20" s="79"/>
+      <c r="B20" s="79"/>
       <c r="C20" s="43" t="s">
         <v>102</v>
       </c>
@@ -4620,10 +4606,10 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="75" t="s">
+      <c r="A30" s="78" t="s">
         <v>244</v>
       </c>
-      <c r="B30" s="75" t="s">
+      <c r="B30" s="78" t="s">
         <v>115</v>
       </c>
       <c r="C30" s="42" t="s">
@@ -4647,8 +4633,8 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="76"/>
-      <c r="B32" s="76"/>
+      <c r="A32" s="79"/>
+      <c r="B32" s="79"/>
       <c r="C32" s="43" t="s">
         <v>118</v>
       </c>
@@ -4999,10 +4985,10 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="77" t="s">
+      <c r="A8" s="75" t="s">
         <v>108</v>
       </c>
-      <c r="B8" s="77" t="s">
+      <c r="B8" s="75" t="s">
         <v>109</v>
       </c>
       <c r="C8" s="37" t="s">
@@ -5013,8 +4999,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="78"/>
-      <c r="B9" s="78"/>
+      <c r="A9" s="76"/>
+      <c r="B9" s="76"/>
       <c r="C9" s="38" t="s">
         <v>111</v>
       </c>
@@ -5023,8 +5009,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="79"/>
-      <c r="B10" s="79"/>
+      <c r="A10" s="77"/>
+      <c r="B10" s="77"/>
       <c r="C10" s="39" t="s">
         <v>112</v>
       </c>
@@ -5398,10 +5384,10 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="75" t="s">
+      <c r="A37" s="78" t="s">
         <v>98</v>
       </c>
-      <c r="B37" s="75" t="s">
+      <c r="B37" s="78" t="s">
         <v>100</v>
       </c>
       <c r="C37" s="42" t="s">
@@ -5412,8 +5398,8 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="76"/>
-      <c r="B38" s="76"/>
+      <c r="A38" s="79"/>
+      <c r="B38" s="79"/>
       <c r="C38" s="43" t="s">
         <v>102</v>
       </c>
@@ -5436,10 +5422,10 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="75" t="s">
+      <c r="A40" s="78" t="s">
         <v>136</v>
       </c>
-      <c r="B40" s="75" t="s">
+      <c r="B40" s="78" t="s">
         <v>138</v>
       </c>
       <c r="C40" s="42" t="s">
@@ -5450,8 +5436,8 @@
       </c>
     </row>
     <row r="41" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="76"/>
-      <c r="B41" s="76"/>
+      <c r="A41" s="79"/>
+      <c r="B41" s="79"/>
       <c r="C41" s="43" t="s">
         <v>102</v>
       </c>
@@ -5610,10 +5596,10 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="75" t="s">
         <v>230</v>
       </c>
-      <c r="B4" s="77" t="s">
+      <c r="B4" s="75" t="s">
         <v>211</v>
       </c>
       <c r="C4" s="37" t="s">
@@ -5627,8 +5613,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="79"/>
-      <c r="B5" s="79"/>
+      <c r="A5" s="77"/>
+      <c r="B5" s="77"/>
       <c r="C5" s="39" t="s">
         <v>254</v>
       </c>
@@ -5679,10 +5665,10 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="77" t="s">
+      <c r="A9" s="75" t="s">
         <v>108</v>
       </c>
-      <c r="B9" s="77" t="s">
+      <c r="B9" s="75" t="s">
         <v>109</v>
       </c>
       <c r="C9" s="37" t="s">
@@ -5693,8 +5679,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="78"/>
-      <c r="B10" s="78"/>
+      <c r="A10" s="76"/>
+      <c r="B10" s="76"/>
       <c r="C10" s="38" t="s">
         <v>111</v>
       </c>
@@ -5703,8 +5689,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="79"/>
-      <c r="B11" s="79"/>
+      <c r="A11" s="77"/>
+      <c r="B11" s="77"/>
       <c r="C11" s="39" t="s">
         <v>112</v>
       </c>
@@ -5783,10 +5769,10 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="75" t="s">
+      <c r="A17" s="78" t="s">
         <v>181</v>
       </c>
-      <c r="B17" s="75" t="s">
+      <c r="B17" s="78" t="s">
         <v>183</v>
       </c>
       <c r="C17" s="42" t="s">
@@ -5797,8 +5783,8 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="76"/>
-      <c r="B18" s="76"/>
+      <c r="A18" s="79"/>
+      <c r="B18" s="79"/>
       <c r="C18" s="43" t="s">
         <v>102</v>
       </c>
@@ -6207,18 +6193,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C7" r:id="rId1" display="https://www.ptagis.org/Content/DataSpecification/topics/timestamps.htm" xr:uid="{B214498C-AA54-4E7B-9189-B04B5858FBC5}"/>

</xml_diff>